<commit_message>
Add bValueZeroThreshold and bValueScalingTol
Introduce bValueZeroThreshold and bValueScalingTol parameters to improve handling almost-zero b-values. Further b-vectors are now checked for being close to the unit vector.
</commit_message>
<xml_diff>
--- a/src/structural_pipeline/structuralParameterProperties.xlsx
+++ b/src/structural_pipeline/structuralParameterProperties.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Documents/projects/connectomizer_develop/CATO_REBORN/CATO-utils/CATO/src/structural_pipeline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/GitHub/CATO_public/src/structural_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1BE2D4-7F7A-4C4A-A657-C282FF59137A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3292DF1C-93B9-9544-9AD5-88F6BAF21A1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28620" windowHeight="21600" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="207">
   <si>
     <t>parameter</t>
   </si>
@@ -628,6 +628,24 @@
   </si>
   <si>
     <t>Freesurfer's color lookup table of the template</t>
+  </si>
+  <si>
+    <t>general.bValueZeroThreshold</t>
+  </si>
+  <si>
+    <t>structural_preprocessing,reconstruction_diffusion</t>
+  </si>
+  <si>
+    <t>scalar nonempty nonnegative</t>
+  </si>
+  <si>
+    <t>B-values smaller or equal to this threshold are assumed to indicate b0-scans and set to b-value = 0.</t>
+  </si>
+  <si>
+    <t>general.bValueScalingTol</t>
+  </si>
+  <si>
+    <t>B-vectors with a norm that deviates from 1 more than this threshold are labeled as potentially non-unit gradients.</t>
   </si>
 </sst>
 </file>
@@ -991,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601D286D-EE53-F94C-94B6-2BBF9957A3E8}">
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F33" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1002,8 +1020,8 @@
     <col min="1" max="1" width="46" customWidth="1"/>
     <col min="2" max="2" width="33.83203125" customWidth="1"/>
     <col min="3" max="3" width="47.5" customWidth="1"/>
-    <col min="4" max="4" width="0.6640625" customWidth="1"/>
-    <col min="5" max="5" width="1.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
     <col min="6" max="6" width="36" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" style="1" customWidth="1"/>
   </cols>
@@ -1216,70 +1234,70 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
+        <v>201</v>
+      </c>
+      <c r="D11" t="s">
+        <v>202</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>81</v>
+        <v>203</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>144</v>
+        <v>190</v>
       </c>
       <c r="H11" t="s">
-        <v>152</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>119</v>
+        <v>205</v>
+      </c>
+      <c r="D12" t="s">
+        <v>202</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>80</v>
+        <v>203</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>144</v>
+        <v>190</v>
       </c>
       <c r="H12" t="s">
-        <v>97</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
         <v>74</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H13" t="s">
-        <v>98</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>119</v>
       </c>
       <c r="E14" t="s">
         <v>74</v>
@@ -1291,15 +1309,15 @@
         <v>144</v>
       </c>
       <c r="H14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
       </c>
       <c r="E15" t="s">
         <v>74</v>
@@ -1311,12 +1329,12 @@
         <v>144</v>
       </c>
       <c r="H15" t="s">
-        <v>153</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -1325,18 +1343,18 @@
         <v>74</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H16" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -1351,92 +1369,92 @@
         <v>144</v>
       </c>
       <c r="H17" t="s">
-        <v>100</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>189</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D18" t="s">
-        <v>139</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>4</v>
+        <v>74</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" t="s">
-        <v>67</v>
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H19" t="s">
-        <v>197</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
+        <v>189</v>
+      </c>
+      <c r="C20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" t="s">
+        <v>139</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H20" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
+        <v>134</v>
+      </c>
+      <c r="D21" t="s">
+        <v>67</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H21" t="s">
-        <v>102</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -1451,29 +1469,32 @@
         <v>144</v>
       </c>
       <c r="H22" t="s">
-        <v>156</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>4</v>
+        <v>74</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H23" t="s">
-        <v>157</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
@@ -1481,16 +1502,19 @@
       <c r="E24" t="s">
         <v>74</v>
       </c>
+      <c r="F24" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="G24" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
@@ -1498,128 +1522,116 @@
       <c r="E25" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="G25" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H25" t="s">
-        <v>103</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>138</v>
-      </c>
-      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
         <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
         <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>138</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H28" t="s">
-        <v>105</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s">
         <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H29" t="s">
-        <v>160</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" t="s">
-        <v>133</v>
-      </c>
-      <c r="C30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" t="s">
         <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H30" t="s">
-        <v>161</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
@@ -1634,15 +1646,15 @@
         <v>144</v>
       </c>
       <c r="H31" t="s">
-        <v>106</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>133</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
@@ -1657,12 +1669,15 @@
         <v>144</v>
       </c>
       <c r="H32" t="s">
-        <v>107</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -1677,12 +1692,15 @@
         <v>144</v>
       </c>
       <c r="H33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
@@ -1697,15 +1715,12 @@
         <v>144</v>
       </c>
       <c r="H34" t="s">
-        <v>162</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
@@ -1720,15 +1735,12 @@
         <v>144</v>
       </c>
       <c r="H35" t="s">
-        <v>163</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
@@ -1743,35 +1755,41 @@
         <v>144</v>
       </c>
       <c r="H36" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>122</v>
-      </c>
-      <c r="D37" t="s">
-        <v>57</v>
+        <v>30</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>123</v>
+        <v>74</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H37" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="E38" t="s">
         <v>74</v>
@@ -1783,35 +1801,32 @@
         <v>144</v>
       </c>
       <c r="H38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" t="s">
         <v>57</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H39" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="C40" t="s">
         <v>57</v>
@@ -1826,17 +1841,14 @@
         <v>144</v>
       </c>
       <c r="H40" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" t="s">
         <v>57</v>
       </c>
       <c r="E41" t="s">
@@ -1849,16 +1861,19 @@
         <v>144</v>
       </c>
       <c r="H41" t="s">
-        <v>109</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
         <v>56</v>
       </c>
+      <c r="C42" t="s">
+        <v>57</v>
+      </c>
       <c r="E42" t="s">
         <v>74</v>
       </c>
@@ -1869,16 +1884,19 @@
         <v>144</v>
       </c>
       <c r="H42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
         <v>56</v>
       </c>
+      <c r="C43" t="s">
+        <v>57</v>
+      </c>
       <c r="E43" t="s">
         <v>74</v>
       </c>
@@ -1889,17 +1907,14 @@
         <v>144</v>
       </c>
       <c r="H43" t="s">
-        <v>200</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" t="s">
         <v>56</v>
       </c>
       <c r="E44" t="s">
@@ -1912,46 +1927,55 @@
         <v>144</v>
       </c>
       <c r="H44" t="s">
-        <v>199</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" t="s">
-        <v>2</v>
+        <v>64</v>
+      </c>
+      <c r="B45" t="s">
+        <v>56</v>
       </c>
       <c r="E45" t="s">
-        <v>3</v>
+        <v>74</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H45" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" t="s">
-        <v>2</v>
+        <v>65</v>
+      </c>
+      <c r="B46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" t="s">
+        <v>56</v>
       </c>
       <c r="E46" t="s">
-        <v>3</v>
+        <v>74</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H46" t="s">
-        <v>168</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D47" t="s">
         <v>2</v>
@@ -1959,19 +1983,16 @@
       <c r="E47" t="s">
         <v>3</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="G47" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H47" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D48" t="s">
         <v>2</v>
@@ -1979,19 +2000,16 @@
       <c r="E48" t="s">
         <v>3</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="G48" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H48" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D49" t="s">
         <v>2</v>
@@ -2006,12 +2024,12 @@
         <v>144</v>
       </c>
       <c r="H49" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D50" t="s">
         <v>2</v>
@@ -2020,18 +2038,18 @@
         <v>3</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H50" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D51" t="s">
         <v>2</v>
@@ -2046,12 +2064,12 @@
         <v>144</v>
       </c>
       <c r="H51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D52" t="s">
         <v>2</v>
@@ -2060,18 +2078,18 @@
         <v>3</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H52" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D53" t="s">
         <v>2</v>
@@ -2086,12 +2104,12 @@
         <v>144</v>
       </c>
       <c r="H53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D54" t="s">
         <v>2</v>
@@ -2106,12 +2124,12 @@
         <v>144</v>
       </c>
       <c r="H54" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D55" t="s">
         <v>2</v>
@@ -2125,13 +2143,13 @@
       <c r="G55" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H55" s="4" t="s">
-        <v>174</v>
+      <c r="H55" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D56" t="s">
         <v>2</v>
@@ -2146,12 +2164,12 @@
         <v>144</v>
       </c>
       <c r="H56" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D57" t="s">
         <v>2</v>
@@ -2165,13 +2183,13 @@
       <c r="G57" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H57" t="s">
-        <v>172</v>
+      <c r="H57" s="4" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D58" t="s">
         <v>2</v>
@@ -2186,193 +2204,193 @@
         <v>144</v>
       </c>
       <c r="H58" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>45</v>
-      </c>
-      <c r="B59" t="s">
-        <v>67</v>
-      </c>
-      <c r="C59" t="s">
+        <v>43</v>
+      </c>
+      <c r="D59" t="s">
         <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H59" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>46</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C60" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" t="s">
         <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H60" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>126</v>
-      </c>
-      <c r="B61" s="1"/>
-      <c r="D61" t="s">
+        <v>45</v>
+      </c>
+      <c r="B61" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" t="s">
         <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>123</v>
+        <v>74</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H61" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>127</v>
-      </c>
-      <c r="B62" s="1"/>
-      <c r="D62" t="s">
+        <v>46</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C62" t="s">
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H62" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B63" s="1"/>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>74</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H63" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>129</v>
-      </c>
-      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+      <c r="B64" s="1"/>
+      <c r="D64" t="s">
         <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>123</v>
+        <v>77</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H64" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B65" s="1"/>
+      <c r="C65" t="s">
+        <v>2</v>
+      </c>
       <c r="E65" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H65" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>47</v>
-      </c>
-      <c r="D66" t="s">
-        <v>67</v>
+        <v>129</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>3</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>87</v>
+        <v>123</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H66" t="s">
-        <v>112</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>48</v>
-      </c>
-      <c r="D67" t="s">
-        <v>67</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="B67" s="1"/>
       <c r="E67" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H67" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>47</v>
       </c>
       <c r="D68" t="s">
         <v>67</v>
@@ -2381,18 +2399,18 @@
         <v>3</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H68" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D69" t="s">
         <v>67</v>
@@ -2401,18 +2419,18 @@
         <v>3</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H69" t="s">
-        <v>113</v>
+        <v>194</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>50</v>
+        <v>132</v>
       </c>
       <c r="D70" t="s">
         <v>67</v>
@@ -2420,16 +2438,19 @@
       <c r="E70" t="s">
         <v>3</v>
       </c>
+      <c r="F70" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="G70" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H70" t="s">
-        <v>195</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D71" t="s">
         <v>67</v>
@@ -2437,16 +2458,19 @@
       <c r="E71" t="s">
         <v>3</v>
       </c>
+      <c r="F71" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="G71" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H71" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D72" t="s">
         <v>67</v>
@@ -2454,65 +2478,59 @@
       <c r="E72" t="s">
         <v>3</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="G72" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H72" t="s">
-        <v>115</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>53</v>
-      </c>
-      <c r="B73" t="s">
-        <v>58</v>
-      </c>
-      <c r="C73" t="s">
+        <v>51</v>
+      </c>
+      <c r="D73" t="s">
         <v>67</v>
       </c>
       <c r="E73" t="s">
-        <v>74</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H73" t="s">
-        <v>183</v>
+        <v>114</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>124</v>
+        <v>52</v>
       </c>
       <c r="D74" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E74" t="s">
-        <v>123</v>
+        <v>3</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>190</v>
+        <v>144</v>
       </c>
       <c r="H74" t="s">
-        <v>184</v>
+        <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C75" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E75" t="s">
         <v>74</v>
@@ -2524,52 +2542,52 @@
         <v>144</v>
       </c>
       <c r="H75" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D76" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E76" t="s">
-        <v>3</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>144</v>
+        <v>190</v>
       </c>
       <c r="H76" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>79</v>
-      </c>
-      <c r="D77" t="s">
+        <v>54</v>
+      </c>
+      <c r="B77" t="s">
         <v>59</v>
       </c>
+      <c r="C77" t="s">
+        <v>58</v>
+      </c>
       <c r="E77" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H77" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="D78" t="s">
         <v>59</v>
@@ -2578,32 +2596,72 @@
         <v>3</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H78" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>79</v>
+      </c>
+      <c r="D79" t="s">
+        <v>59</v>
+      </c>
+      <c r="E79" t="s">
+        <v>3</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H79" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>78</v>
+      </c>
+      <c r="D80" t="s">
+        <v>59</v>
+      </c>
+      <c r="E80" t="s">
+        <v>3</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H80" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>55</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C81" t="s">
         <v>59</v>
       </c>
-      <c r="E79" t="s">
-        <v>74</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H79" t="s">
+      <c r="E81" t="s">
+        <v>74</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H81" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Additional edits to update ROIs matching
</commit_message>
<xml_diff>
--- a/src/structural_pipeline/structuralParameterProperties.xlsx
+++ b/src/structural_pipeline/structuralParameterProperties.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siemon/Documents/GitHub/CATO_public/src/structural_pipeline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Documents/projects/connectomizer_develop/CATO_public/src/structural_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A9D715-E916-6943-89DA-C469A9099E5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA4D272-FECD-9948-B02D-F16EFDB6442F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31300" windowHeight="21600" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="210">
   <si>
     <t>parameter</t>
   </si>
@@ -418,9 +418,6 @@
   </si>
   <si>
     <t>reconstruction_diffusion.gradientNonlinearities.nonlinearitiesFile</t>
-  </si>
-  <si>
-    <t>isfile</t>
   </si>
   <si>
     <t>reconstruction_fibers.minFA</t>
@@ -1023,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601D286D-EE53-F94C-94B6-2BBF9957A3E8}">
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1058,10 +1055,10 @@
         <v>16</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1078,10 +1075,10 @@
         <v>80</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1098,15 +1095,15 @@
         <v>80</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -1115,13 +1112,13 @@
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1138,10 +1135,10 @@
         <v>5</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1158,10 +1155,10 @@
         <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1175,13 +1172,13 @@
         <v>77</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1198,10 +1195,10 @@
         <v>5</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1215,21 +1212,21 @@
         <v>73</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" t="s">
         <v>135</v>
-      </c>
-      <c r="D10" t="s">
-        <v>136</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -1238,50 +1235,50 @@
         <v>5</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>200</v>
+      </c>
+      <c r="D11" t="s">
         <v>201</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H11" t="s">
         <v>203</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="H11" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H12" t="s">
         <v>205</v>
-      </c>
-      <c r="D12" t="s">
-        <v>202</v>
-      </c>
-      <c r="E12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="H12" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1298,10 +1295,10 @@
         <v>81</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1318,7 +1315,7 @@
         <v>80</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H14" t="s">
         <v>97</v>
@@ -1338,7 +1335,7 @@
         <v>82</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H15" t="s">
         <v>98</v>
@@ -1358,7 +1355,7 @@
         <v>80</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H16" t="s">
         <v>99</v>
@@ -1378,10 +1375,10 @@
         <v>82</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1398,10 +1395,10 @@
         <v>82</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1418,7 +1415,7 @@
         <v>82</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H19" t="s">
         <v>100</v>
@@ -1426,27 +1423,27 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D21" t="s">
         <v>67</v>
@@ -1458,10 +1455,10 @@
         <v>89</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1478,7 +1475,7 @@
         <v>82</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H22" t="s">
         <v>101</v>
@@ -1498,7 +1495,7 @@
         <v>82</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H23" t="s">
         <v>102</v>
@@ -1518,10 +1515,10 @@
         <v>82</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1535,10 +1532,10 @@
         <v>4</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1552,10 +1549,10 @@
         <v>74</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1572,7 +1569,7 @@
         <v>82</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H27" t="s">
         <v>103</v>
@@ -1580,7 +1577,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -1592,10 +1589,10 @@
         <v>5</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1612,7 +1609,7 @@
         <v>83</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H29" t="s">
         <v>104</v>
@@ -1632,7 +1629,7 @@
         <v>84</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H30" t="s">
         <v>105</v>
@@ -1655,10 +1652,10 @@
         <v>82</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1666,7 +1663,7 @@
         <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
@@ -1678,10 +1675,10 @@
         <v>82</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1701,7 +1698,7 @@
         <v>82</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H33" t="s">
         <v>106</v>
@@ -1724,7 +1721,7 @@
         <v>82</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H34" t="s">
         <v>107</v>
@@ -1744,7 +1741,7 @@
         <v>82</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H35" t="s">
         <v>108</v>
@@ -1764,10 +1761,10 @@
         <v>82</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1787,10 +1784,10 @@
         <v>82</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1810,10 +1807,10 @@
         <v>82</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1827,10 +1824,10 @@
         <v>123</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H39" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1850,10 +1847,10 @@
         <v>82</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1870,15 +1867,15 @@
         <v>82</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D42" t="s">
         <v>57</v>
@@ -1886,20 +1883,23 @@
       <c r="E42" t="s">
         <v>123</v>
       </c>
+      <c r="F42" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G42" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H42" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>207</v>
+      </c>
+      <c r="B43" t="s">
         <v>208</v>
       </c>
-      <c r="B43" t="s">
-        <v>209</v>
-      </c>
       <c r="E43" t="s">
         <v>74</v>
       </c>
@@ -1907,10 +1907,10 @@
         <v>82</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H43" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1930,7 +1930,7 @@
         <v>82</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H44" t="s">
         <v>110</v>
@@ -1953,7 +1953,7 @@
         <v>82</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H45" t="s">
         <v>109</v>
@@ -1973,7 +1973,7 @@
         <v>82</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H46" t="s">
         <v>111</v>
@@ -1993,10 +1993,10 @@
         <v>82</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H47" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -2016,10 +2016,10 @@
         <v>82</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H48" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -2033,10 +2033,10 @@
         <v>3</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -2050,10 +2050,10 @@
         <v>3</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H50" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -2070,10 +2070,10 @@
         <v>85</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H51" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -2090,10 +2090,10 @@
         <v>85</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H52" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -2110,10 +2110,10 @@
         <v>85</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H53" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -2130,10 +2130,10 @@
         <v>86</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H54" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -2150,10 +2150,10 @@
         <v>85</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H55" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -2170,10 +2170,10 @@
         <v>85</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H56" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2190,10 +2190,10 @@
         <v>85</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H57" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2210,10 +2210,10 @@
         <v>85</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2230,10 +2230,10 @@
         <v>85</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2250,10 +2250,10 @@
         <v>85</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H60" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -2270,10 +2270,10 @@
         <v>85</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H61" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -2290,10 +2290,10 @@
         <v>85</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H62" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -2313,10 +2313,10 @@
         <v>82</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -2324,7 +2324,7 @@
         <v>46</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C64" t="s">
         <v>2</v>
@@ -2336,10 +2336,10 @@
         <v>82</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2353,11 +2353,14 @@
       <c r="E65" t="s">
         <v>123</v>
       </c>
+      <c r="F65" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G65" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H65" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2375,10 +2378,10 @@
         <v>5</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H66" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2396,45 +2399,47 @@
         <v>82</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H67" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>129</v>
       </c>
-      <c r="B68" t="s">
+      <c r="D68" t="s">
         <v>2</v>
       </c>
       <c r="E68" t="s">
         <v>123</v>
       </c>
+      <c r="F68" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G68" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H68" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>130</v>
       </c>
-      <c r="B69" s="1"/>
+      <c r="B69" t="s">
+        <v>2</v>
+      </c>
       <c r="E69" t="s">
         <v>4</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="G69" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H69" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -2451,7 +2456,7 @@
         <v>87</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H70" t="s">
         <v>112</v>
@@ -2471,15 +2476,15 @@
         <v>88</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H71" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D72" t="s">
         <v>67</v>
@@ -2491,7 +2496,7 @@
         <v>85</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H72" t="s">
         <v>116</v>
@@ -2511,7 +2516,7 @@
         <v>89</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H73" t="s">
         <v>113</v>
@@ -2528,10 +2533,10 @@
         <v>3</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H74" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -2545,7 +2550,7 @@
         <v>3</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H75" t="s">
         <v>114</v>
@@ -2565,7 +2570,7 @@
         <v>86</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H76" t="s">
         <v>115</v>
@@ -2588,10 +2593,10 @@
         <v>82</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H77" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -2605,10 +2610,10 @@
         <v>123</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H78" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -2628,10 +2633,10 @@
         <v>82</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H79" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -2648,10 +2653,10 @@
         <v>88</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H80" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -2668,10 +2673,10 @@
         <v>90</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H81" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -2688,10 +2693,10 @@
         <v>85</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H82" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -2708,7 +2713,7 @@
         <v>82</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H83" t="s">
         <v>117</v>

</xml_diff>

<commit_message>
Remove old parameter from parameters file
</commit_message>
<xml_diff>
--- a/src/structural_pipeline/structuralParameterProperties.xlsx
+++ b/src/structural_pipeline/structuralParameterProperties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Documents/projects/connectomizer_develop/CATO_public/src/structural_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA4D272-FECD-9948-B02D-F16EFDB6442F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31F5AF0-9CB9-B04F-8D74-3A59461D87A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="31300" windowHeight="21600" xr2:uid="{CCB64B25-1A8A-5846-9EBF-37D23491F92D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="209">
   <si>
     <t>parameter</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>collect_region_properties.statsSubFile</t>
-  </si>
-  <si>
-    <t>collect_region_properties.lutFile</t>
   </si>
   <si>
     <t>collect_region_properties.regionPropertiesFile</t>
@@ -1018,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601D286D-EE53-F94C-94B6-2BBF9957A3E8}">
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1037,13 +1034,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -1055,10 +1052,10 @@
         <v>16</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1072,13 +1069,13 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1092,18 +1089,18 @@
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -1115,15 +1112,15 @@
         <v>5</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -1135,15 +1132,15 @@
         <v>5</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -1155,10 +1152,10 @@
         <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1169,36 +1166,36 @@
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1209,24 +1206,24 @@
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" t="s">
         <v>134</v>
-      </c>
-      <c r="D10" t="s">
-        <v>135</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -1235,50 +1232,50 @@
         <v>5</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" t="s">
         <v>200</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H11" t="s">
         <v>202</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="H11" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>203</v>
+      </c>
+      <c r="D12" t="s">
+        <v>200</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H12" t="s">
         <v>204</v>
-      </c>
-      <c r="D12" t="s">
-        <v>201</v>
-      </c>
-      <c r="E12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="H12" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1289,16 +1286,16 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1306,19 +1303,19 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1326,19 +1323,19 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1349,16 +1346,16 @@
         <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1369,16 +1366,16 @@
         <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1389,16 +1386,16 @@
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1409,121 +1406,121 @@
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" t="s">
         <v>3</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
@@ -1532,27 +1529,27 @@
         <v>4</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1566,18 +1563,18 @@
         <v>4</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -1589,10 +1586,10 @@
         <v>5</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1606,13 +1603,13 @@
         <v>3</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1626,18 +1623,18 @@
         <v>3</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s">
         <v>57</v>
@@ -1646,39 +1643,39 @@
         <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1692,16 +1689,16 @@
         <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1715,16 +1712,16 @@
         <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1735,16 +1732,16 @@
         <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1755,16 +1752,16 @@
         <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1778,16 +1775,16 @@
         <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1795,62 +1792,62 @@
         <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
         <v>11</v>
       </c>
       <c r="E38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D39" t="s">
         <v>57</v>
       </c>
       <c r="E39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" t="s">
         <v>71</v>
-      </c>
-      <c r="B40" t="s">
-        <v>72</v>
       </c>
       <c r="C40" t="s">
         <v>57</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1861,56 +1858,56 @@
         <v>57</v>
       </c>
       <c r="E41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D42" t="s">
         <v>57</v>
       </c>
       <c r="E42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>206</v>
+      </c>
+      <c r="B43" t="s">
         <v>207</v>
       </c>
-      <c r="B43" t="s">
-        <v>208</v>
-      </c>
       <c r="E43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H43" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1924,16 +1921,16 @@
         <v>57</v>
       </c>
       <c r="E44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1947,16 +1944,16 @@
         <v>57</v>
       </c>
       <c r="E45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -1967,16 +1964,16 @@
         <v>56</v>
       </c>
       <c r="E46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -1984,47 +1981,44 @@
         <v>64</v>
       </c>
       <c r="B47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" t="s">
         <v>56</v>
       </c>
       <c r="E47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H47" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>65</v>
-      </c>
-      <c r="B48" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48" t="s">
-        <v>56</v>
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>74</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H48" t="s">
-        <v>198</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D49" t="s">
         <v>2</v>
@@ -2033,7 +2027,7 @@
         <v>3</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H49" t="s">
         <v>166</v>
@@ -2041,7 +2035,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D50" t="s">
         <v>2</v>
@@ -2049,16 +2043,19 @@
       <c r="E50" t="s">
         <v>3</v>
       </c>
+      <c r="F50" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="G50" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H50" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D51" t="s">
         <v>2</v>
@@ -2067,18 +2064,18 @@
         <v>3</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H51" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D52" t="s">
         <v>2</v>
@@ -2087,10 +2084,10 @@
         <v>3</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H52" t="s">
         <v>168</v>
@@ -2098,7 +2095,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D53" t="s">
         <v>2</v>
@@ -2110,15 +2107,15 @@
         <v>85</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H53" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D54" t="s">
         <v>2</v>
@@ -2127,18 +2124,18 @@
         <v>3</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H54" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D55" t="s">
         <v>2</v>
@@ -2147,18 +2144,18 @@
         <v>3</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H55" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D56" t="s">
         <v>2</v>
@@ -2167,18 +2164,18 @@
         <v>3</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H56" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D57" t="s">
         <v>2</v>
@@ -2187,10 +2184,10 @@
         <v>3</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H57" t="s">
         <v>171</v>
@@ -2198,7 +2195,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D58" t="s">
         <v>2</v>
@@ -2207,18 +2204,18 @@
         <v>3</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H58" t="s">
+        <v>142</v>
+      </c>
+      <c r="H58" s="4" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D59" t="s">
         <v>2</v>
@@ -2227,18 +2224,18 @@
         <v>3</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H59" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H59" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D60" t="s">
         <v>2</v>
@@ -2247,18 +2244,18 @@
         <v>3</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H60" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D61" t="s">
         <v>2</v>
@@ -2267,10 +2264,10 @@
         <v>3</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H61" t="s">
         <v>171</v>
@@ -2278,42 +2275,45 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>44</v>
-      </c>
-      <c r="D62" t="s">
+        <v>45</v>
+      </c>
+      <c r="B62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" t="s">
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H62" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>45</v>
-      </c>
-      <c r="B63" t="s">
-        <v>67</v>
+        <v>46</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="C63" t="s">
         <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H63" t="s">
         <v>175</v>
@@ -2321,22 +2321,20 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>46</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C64" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" s="1"/>
+      <c r="D64" t="s">
         <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H64" t="s">
         <v>176</v>
@@ -2351,13 +2349,13 @@
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>123</v>
+        <v>76</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H65" t="s">
         <v>177</v>
@@ -2368,17 +2366,17 @@
         <v>127</v>
       </c>
       <c r="B66" s="1"/>
-      <c r="D66" t="s">
+      <c r="C66" t="s">
         <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H66" t="s">
         <v>178</v>
@@ -2388,18 +2386,17 @@
       <c r="A67" t="s">
         <v>128</v>
       </c>
-      <c r="B67" s="1"/>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H67" t="s">
         <v>179</v>
@@ -2409,17 +2406,14 @@
       <c r="A68" t="s">
         <v>129</v>
       </c>
-      <c r="D68" t="s">
+      <c r="B68" t="s">
         <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>123</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H68" t="s">
         <v>180</v>
@@ -2427,27 +2421,30 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>130</v>
-      </c>
-      <c r="B69" t="s">
-        <v>2</v>
+        <v>47</v>
+      </c>
+      <c r="D69" t="s">
+        <v>66</v>
       </c>
       <c r="E69" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H69" t="s">
-        <v>181</v>
+        <v>111</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E70" t="s">
         <v>3</v>
@@ -2456,101 +2453,101 @@
         <v>87</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H70" t="s">
-        <v>112</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>48</v>
+        <v>130</v>
       </c>
       <c r="D71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E71" t="s">
         <v>3</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H71" t="s">
-        <v>193</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>131</v>
+        <v>49</v>
       </c>
       <c r="D72" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E72" t="s">
         <v>3</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H72" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D73" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E73" t="s">
         <v>3</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="G73" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H73" t="s">
-        <v>113</v>
+        <v>193</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E74" t="s">
         <v>3</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H74" t="s">
-        <v>194</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D75" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E75" t="s">
         <v>3</v>
       </c>
+      <c r="F75" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="G75" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H75" t="s">
         <v>114</v>
@@ -2558,42 +2555,39 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>52</v>
-      </c>
-      <c r="D76" t="s">
-        <v>67</v>
+        <v>53</v>
+      </c>
+      <c r="B76" t="s">
+        <v>58</v>
+      </c>
+      <c r="C76" t="s">
+        <v>66</v>
       </c>
       <c r="E76" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H76" t="s">
-        <v>115</v>
+        <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>53</v>
-      </c>
-      <c r="B77" t="s">
+        <v>123</v>
+      </c>
+      <c r="D77" t="s">
         <v>58</v>
       </c>
-      <c r="C77" t="s">
-        <v>67</v>
-      </c>
       <c r="E77" t="s">
-        <v>74</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>143</v>
+        <v>188</v>
       </c>
       <c r="H77" t="s">
         <v>182</v>
@@ -2601,16 +2595,22 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>124</v>
-      </c>
-      <c r="D78" t="s">
+        <v>54</v>
+      </c>
+      <c r="B78" t="s">
+        <v>59</v>
+      </c>
+      <c r="C78" t="s">
         <v>58</v>
       </c>
       <c r="E78" t="s">
-        <v>123</v>
+        <v>73</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>189</v>
+        <v>142</v>
       </c>
       <c r="H78" t="s">
         <v>183</v>
@@ -2618,30 +2618,27 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>54</v>
-      </c>
-      <c r="B79" t="s">
+        <v>119</v>
+      </c>
+      <c r="D79" t="s">
         <v>59</v>
       </c>
-      <c r="C79" t="s">
-        <v>58</v>
-      </c>
       <c r="E79" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H79" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="D80" t="s">
         <v>59</v>
@@ -2650,18 +2647,18 @@
         <v>3</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H80" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D81" t="s">
         <v>59</v>
@@ -2670,53 +2667,33 @@
         <v>3</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H81" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>78</v>
-      </c>
-      <c r="D82" t="s">
+        <v>55</v>
+      </c>
+      <c r="C82" t="s">
         <v>59</v>
       </c>
       <c r="E82" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H82" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>55</v>
-      </c>
-      <c r="C83" t="s">
-        <v>59</v>
-      </c>
-      <c r="E83" t="s">
-        <v>74</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H83" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>